<commit_message>
Fixing parameters that save the metrics
</commit_message>
<xml_diff>
--- a/2-4 GHz Analysis/tables/models_metrics_in_test_set.xlsx
+++ b/2-4 GHz Analysis/tables/models_metrics_in_test_set.xlsx
@@ -465,7 +465,7 @@
         <v>3.857379000515782</v>
       </c>
       <c r="C2" t="n">
-        <v>3.857379000515782</v>
+        <v>3.803205503849247</v>
       </c>
       <c r="D2" t="n">
         <v>-0.8142503611526666</v>
@@ -481,7 +481,7 @@
         <v>1.408999750282552</v>
       </c>
       <c r="C3" t="n">
-        <v>1.408999750282552</v>
+        <v>1.175777777777777</v>
       </c>
       <c r="D3" t="n">
         <v>0.7579336471916457</v>

</xml_diff>